<commit_message>
Edit to BOM and Summary
</commit_message>
<xml_diff>
--- a/Documentation/Working_Documents/Bottle_Opener_BOM_V1.0.xlsx
+++ b/Documentation/Working_Documents/Bottle_Opener_BOM_V1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neilsquiresoc.sharepoint.com/sites/MMC-Team/Shared Documents/Server/3 AT Library/WIP/Bottle Opener/GitHub/Documentation/Working_Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="81" documentId="11_DC0E2523FAFE28515E8D5C5A1D4A6B02C3B15AFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A30AF51-9E81-443C-8F2B-808D5FE0CE8D}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="11_DC0E2523FAFE28515E8D5C5A1D4A6B02C3B15AFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F838E101-7F90-4FF7-9689-13E3810102E1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Total Cost</t>
   </si>
@@ -130,6 +130,9 @@
   <si>
     <t>STL file for full functional bottle opener with nominal diameter of approx. 30 mm.</t>
   </si>
+  <si>
+    <t>Bottle-Opener/Build_Files at main · makersmakingchange/Bottle-Opener (github.com)</t>
+  </si>
 </sst>
 </file>
 
@@ -139,7 +142,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,12 +216,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -268,7 +265,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -358,6 +355,15 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -369,7 +375,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1"/>
@@ -381,7 +387,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -396,6 +401,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="60% - Accent4" xfId="3" builtinId="44"/>
@@ -698,7 +709,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -731,7 +742,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="10" t="s">
@@ -741,7 +752,7 @@
         <f>SUM(G3:G3)+E10</f>
         <v>4.6499999999999995</v>
       </c>
-      <c r="D2" s="18">
+      <c r="D2" s="17">
         <f>SUM(F5:F5)/60</f>
         <v>3.7833333333333332</v>
       </c>
@@ -751,22 +762,22 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="21">
+      <c r="B3" s="20">
         <v>25</v>
       </c>
       <c r="E3" s="9"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
       <c r="L3" s="8"/>
     </row>
     <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="19" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -775,7 +786,7 @@
       <c r="D4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="12" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="7" t="s">
@@ -786,10 +797,10 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="21" t="s">
         <v>20</v>
       </c>
       <c r="C5">
@@ -798,20 +809,22 @@
       <c r="D5">
         <v>37</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="13">
         <f>(D5/1000)*$B$3</f>
         <v>0.92499999999999993</v>
       </c>
       <c r="F5">
         <v>227</v>
       </c>
-      <c r="G5" s="8"/>
+      <c r="G5" s="23" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="21" t="s">
         <v>20</v>
       </c>
       <c r="C6">
@@ -820,20 +833,20 @@
       <c r="D6">
         <v>36</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="13">
         <f t="shared" ref="E6:E9" si="0">(D6/1000)*$B$3</f>
         <v>0.89999999999999991</v>
       </c>
       <c r="F6">
         <v>224</v>
       </c>
-      <c r="G6" s="11"/>
+      <c r="G6" s="24"/>
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="21" t="s">
         <v>20</v>
       </c>
       <c r="C7">
@@ -842,19 +855,20 @@
       <c r="D7">
         <v>36</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="13">
         <f t="shared" si="0"/>
         <v>0.89999999999999991</v>
       </c>
       <c r="F7">
         <v>226</v>
       </c>
+      <c r="G7" s="24"/>
     </row>
     <row r="8" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="21" t="s">
         <v>20</v>
       </c>
       <c r="C8">
@@ -863,19 +877,20 @@
       <c r="D8">
         <v>38</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="13">
         <f t="shared" si="0"/>
         <v>0.95</v>
       </c>
       <c r="F8">
         <v>231</v>
       </c>
+      <c r="G8" s="24"/>
     </row>
     <row r="9" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="21" t="s">
         <v>20</v>
       </c>
       <c r="C9">
@@ -884,37 +899,46 @@
       <c r="D9">
         <v>39</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="13">
         <f t="shared" si="0"/>
         <v>0.97499999999999998</v>
       </c>
       <c r="F9">
         <v>241</v>
       </c>
+      <c r="G9" s="24"/>
     </row>
     <row r="10" spans="1:12" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="15">
         <f>SUM(E5:E9)</f>
         <v>4.6499999999999995</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G5:G9"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G5" r:id="rId1" display="https://github.com/makersmakingchange/Bottle-Opener/tree/main/Build_Files" xr:uid="{A3530CF0-E148-4A9D-8D64-AE1EA0AF7D59}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="38b325e6-602c-452a-8617-173bf47082c5" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8cf100d1-0775-4feb-8634-62999c4541bc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1155,20 +1179,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="38b325e6-602c-452a-8617-173bf47082c5" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8cf100d1-0775-4feb-8634-62999c4541bc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="38b325e6-602c-452a-8617-173bf47082c5"/>
+    <ds:schemaRef ds:uri="8cf100d1-0775-4feb-8634-62999c4541bc"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1193,12 +1218,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="38b325e6-602c-452a-8617-173bf47082c5"/>
-    <ds:schemaRef ds:uri="8cf100d1-0775-4feb-8634-62999c4541bc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>